<commit_message>
Add drag & lift values to excel sheet
</commit_message>
<xml_diff>
--- a/Power & Propulsion System/Power Consumption.xlsx
+++ b/Power & Propulsion System/Power Consumption.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\Videos\UAS_Challenge\Power &amp; Propulsion System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77447001-8994-4916-A3DC-A9AA0EB2F7AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5299C4C2-CB7A-41C7-BB70-631BD7024345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Drag &amp; Lift" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Vertical Flight Power</t>
   </si>
@@ -52,6 +53,15 @@
   </si>
   <si>
     <t>Pump</t>
+  </si>
+  <si>
+    <t>Airspeed (m/s)</t>
+  </si>
+  <si>
+    <t>Lift (N)</t>
+  </si>
+  <si>
+    <t>Drag (N)</t>
   </si>
 </sst>
 </file>
@@ -371,7 +381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -428,4 +438,91 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DCE7B62-FB69-4347-8AA6-5823B55756E6}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.1796875" customWidth="1"/>
+    <col min="2" max="2" width="12.90625" customWidth="1"/>
+    <col min="3" max="3" width="13.7265625" customWidth="1"/>
+    <col min="4" max="5" width="8.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>4.8</v>
+      </c>
+      <c r="C3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>47.5</v>
+      </c>
+      <c r="C5">
+        <v>5.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>86.4</v>
+      </c>
+      <c r="C6">
+        <v>9.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modify Power Consumption excel sheet
</commit_message>
<xml_diff>
--- a/Power & Propulsion System/Power Consumption.xlsx
+++ b/Power & Propulsion System/Power Consumption.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\Videos\UAS_Challenge\Power &amp; Propulsion System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCCBB58-BE9F-44A7-BE8C-40F8164BB629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA2D1F0-5FC4-4C64-9DBD-368C6F6A6B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
-    <sheet name="Drag &amp; Lift" sheetId="2" r:id="rId2"/>
+    <sheet name="Power &amp; Thrust Data" sheetId="3" r:id="rId1"/>
+    <sheet name="Drag &amp; Lift Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -430,7 +430,7 @@
   <dimension ref="A1:G80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
@@ -2154,18 +2154,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:B12"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="A2:A23"/>
+    <mergeCell ref="A24:A45"/>
+    <mergeCell ref="B24:B34"/>
+    <mergeCell ref="B35:B45"/>
     <mergeCell ref="A79:A80"/>
     <mergeCell ref="B79:B80"/>
     <mergeCell ref="B46:B56"/>
     <mergeCell ref="B57:B67"/>
     <mergeCell ref="B68:B78"/>
     <mergeCell ref="A46:A78"/>
-    <mergeCell ref="B2:B12"/>
-    <mergeCell ref="B13:B23"/>
-    <mergeCell ref="A2:A23"/>
-    <mergeCell ref="A24:A45"/>
-    <mergeCell ref="B24:B34"/>
-    <mergeCell ref="B35:B45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Calculate Cruise Speed with Payload
</commit_message>
<xml_diff>
--- a/Power & Propulsion System/Power Consumption.xlsx
+++ b/Power & Propulsion System/Power Consumption.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\Videos\UAS_Challenge\Power &amp; Propulsion System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA2D1F0-5FC4-4C64-9DBD-368C6F6A6B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244BC670-9B55-4402-89F9-DE6F0545D541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power &amp; Thrust Data" sheetId="3" r:id="rId1"/>
     <sheet name="Drag &amp; Lift Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Cruise Speed (Loaded)" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Propeller</t>
   </si>
@@ -101,6 +102,30 @@
   </si>
   <si>
     <t>P14*7''</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>Vertical Thrust</t>
+  </si>
+  <si>
+    <t>Horizontal Thrust</t>
+  </si>
+  <si>
+    <t>Total Thrust</t>
+  </si>
+  <si>
+    <t>Thrust per motor</t>
+  </si>
+  <si>
+    <t>Power per Motor</t>
+  </si>
+  <si>
+    <t>Total Power</t>
+  </si>
+  <si>
+    <t>Cruise Efficiency</t>
   </si>
 </sst>
 </file>
@@ -429,9 +454,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{175D03E5-8582-4481-A4D2-A6FC07404F11}">
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B87" sqref="B87"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I73" sqref="I73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -469,7 +494,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -704,7 +729,7 @@
         <v>6.3993166145852456</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
         <v>11</v>
@@ -937,7 +962,7 @@
         <v>5.9703039991426055</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
@@ -1172,7 +1197,7 @@
         <v>5.9308103261478688</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
       <c r="B35" s="1" t="s">
         <v>11</v>
@@ -1440,14 +1465,14 @@
         <v>3.78</v>
       </c>
       <c r="E47">
-        <f t="shared" ref="E47:E67" si="4">D47*C47</f>
+        <f t="shared" ref="E47:E80" si="4">D47*C47</f>
         <v>88.603200000000001</v>
       </c>
       <c r="F47">
         <v>845</v>
       </c>
       <c r="G47">
-        <f t="shared" ref="G47:G67" si="5">F47/E47</f>
+        <f t="shared" ref="G47:G80" si="5">F47/E47</f>
         <v>9.5369016017480188</v>
       </c>
     </row>
@@ -1640,7 +1665,7 @@
         <v>5.6614741453736395</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1"/>
       <c r="B57" s="1" t="s">
         <v>16</v>
@@ -1873,7 +1898,7 @@
         <v>5.625112784216225</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="1"/>
       <c r="B68" s="1" t="s">
         <v>10</v>
@@ -1885,14 +1910,14 @@
         <v>3.71</v>
       </c>
       <c r="E68">
-        <f t="shared" ref="E68:E80" si="6">D68*C68</f>
+        <f t="shared" si="4"/>
         <v>86.962400000000002</v>
       </c>
       <c r="F68">
         <v>917</v>
       </c>
       <c r="G68">
-        <f t="shared" ref="G68:G80" si="7">F68/E68</f>
+        <f t="shared" si="5"/>
         <v>10.544787172387146</v>
       </c>
     </row>
@@ -1906,14 +1931,14 @@
         <v>5.18</v>
       </c>
       <c r="E69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>121.1602</v>
       </c>
       <c r="F69">
         <v>1170</v>
       </c>
       <c r="G69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>9.6566364202105976</v>
       </c>
     </row>
@@ -1927,14 +1952,14 @@
         <v>6.99</v>
       </c>
       <c r="E70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>163.07669999999999</v>
       </c>
       <c r="F70">
         <v>1447</v>
       </c>
       <c r="G70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>8.8731253453129728</v>
       </c>
     </row>
@@ -1948,14 +1973,14 @@
         <v>8.8800000000000008</v>
       </c>
       <c r="E71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>206.54880000000003</v>
       </c>
       <c r="F71">
         <v>1712</v>
       </c>
       <c r="G71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>8.288598142424453</v>
       </c>
     </row>
@@ -1969,14 +1994,14 @@
         <v>10.92</v>
       </c>
       <c r="E72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>253.34399999999999</v>
       </c>
       <c r="F72">
         <v>1963</v>
       </c>
       <c r="G72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>7.7483579638752058</v>
       </c>
     </row>
@@ -1990,14 +2015,14 @@
         <v>13.17</v>
       </c>
       <c r="E73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>304.62209999999999</v>
       </c>
       <c r="F73">
         <v>2230</v>
       </c>
       <c r="G73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>7.3205456859499032</v>
       </c>
     </row>
@@ -2011,14 +2036,14 @@
         <v>15.72</v>
       </c>
       <c r="E74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>362.346</v>
       </c>
       <c r="F74">
         <v>2491</v>
       </c>
       <c r="G74">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>6.8746446766350395</v>
       </c>
     </row>
@@ -2032,14 +2057,14 @@
         <v>18.309999999999999</v>
       </c>
       <c r="E75">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>420.58069999999992</v>
       </c>
       <c r="F75">
         <v>2757</v>
       </c>
       <c r="G75">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>6.5552223390184103</v>
       </c>
     </row>
@@ -2053,14 +2078,14 @@
         <v>21.65</v>
       </c>
       <c r="E76">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>495.13549999999998</v>
       </c>
       <c r="F76">
         <v>3090</v>
       </c>
       <c r="G76">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>6.2407159252366275</v>
       </c>
     </row>
@@ -2074,14 +2099,14 @@
         <v>28.93</v>
       </c>
       <c r="E77">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>655.2645</v>
       </c>
       <c r="F77">
         <v>3697</v>
       </c>
       <c r="G77">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>5.6419964762321166</v>
       </c>
     </row>
@@ -2095,18 +2120,18 @@
         <v>32.83</v>
       </c>
       <c r="E78">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>739.65989999999999</v>
       </c>
       <c r="F78">
         <v>3982</v>
       </c>
       <c r="G78">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>5.3835553340122937</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>17</v>
       </c>
@@ -2120,14 +2145,14 @@
         <v>45</v>
       </c>
       <c r="E79">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>666</v>
       </c>
       <c r="F79">
         <v>2950</v>
       </c>
       <c r="G79">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>4.4294294294294296</v>
       </c>
     </row>
@@ -2141,31 +2166,31 @@
         <v>57.3</v>
       </c>
       <c r="E80">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>829.13099999999997</v>
       </c>
       <c r="F80">
         <v>3680</v>
       </c>
       <c r="G80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>4.4383818721046495</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="B46:B56"/>
+    <mergeCell ref="B57:B67"/>
+    <mergeCell ref="B68:B78"/>
+    <mergeCell ref="A46:A78"/>
     <mergeCell ref="B2:B12"/>
     <mergeCell ref="B13:B23"/>
     <mergeCell ref="A2:A23"/>
     <mergeCell ref="A24:A45"/>
     <mergeCell ref="B24:B34"/>
     <mergeCell ref="B35:B45"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="B46:B56"/>
-    <mergeCell ref="B57:B67"/>
-    <mergeCell ref="B68:B78"/>
-    <mergeCell ref="A46:A78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2176,7 +2201,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2303,4 +2328,1044 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC55B06D-1837-44EB-A9AC-10712F976789}">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="15.54296875" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" customWidth="1"/>
+    <col min="5" max="5" width="19.08984375" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="13.81640625" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>IF(6.9-(0.350317*A2*A2-0.202576*A2)/9.8&gt;0, 6.9-(0.350317*A2*A2-0.202576*A2)/9.8, 0)</f>
+        <v>6.8849243877551025</v>
+      </c>
+      <c r="C2">
+        <f>(0.0350823*A2*A2+0.00372739*A2)/9.8</f>
+        <v>3.960172448979591E-3</v>
+      </c>
+      <c r="D2">
+        <f>SQRT(C2*C2+B2*B2)</f>
+        <v>6.8849255266902336</v>
+      </c>
+      <c r="E2">
+        <f>D2/4</f>
+        <v>1.7212313816725584</v>
+      </c>
+      <c r="F2">
+        <f>1000000*0.0000373344395*E2*E2+ 1000*0.109504955*E2</f>
+        <v>299.09177435095376</v>
+      </c>
+      <c r="G2">
+        <f>F2*4</f>
+        <v>1196.367097403815</v>
+      </c>
+      <c r="H2">
+        <f>F2/A2</f>
+        <v>299.09177435095376</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B22" si="0">IF(6.9-(0.350317*A3*A3-0.202576*A3)/9.8&gt;0, 6.9-(0.350317*A3*A3-0.202576*A3)/9.8, 0)</f>
+        <v>6.7983555102040816</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C22" si="1">(0.0350823*A3*A3+0.00372739*A3)/9.8</f>
+        <v>1.5079997959183671E-2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D31" si="2">SQRT(C3*C3+B3*B3)</f>
+        <v>6.7983722352825486</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E31" si="3">D3/4</f>
+        <v>1.6995930588206372</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F31" si="4">1000000*0.0000373344395*E3*E3+ 1000*0.109504955*E3</f>
+        <v>293.95874183123203</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G31" si="5">F3*4</f>
+        <v>1175.8349673249281</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H31" si="6">F3/A3</f>
+        <v>146.97937091561602</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>6.6402933673469393</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>3.3359476530612241E-2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="2"/>
+        <v>6.6403771624137553</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="3"/>
+        <v>1.6600942906034388</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="4"/>
+        <v>284.6790197586904</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="5"/>
+        <v>1138.7160790347616</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="6"/>
+        <v>94.893006586230129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>6.410737959183674</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>5.8798608163265292E-2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>6.4110076008097501</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="3"/>
+        <v>1.6027519002024375</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="4"/>
+        <v>271.41449264502978</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="5"/>
+        <v>1085.6579705801191</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="6"/>
+        <v>67.853623161257445</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>6.1096892857142864</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>9.1397392857142851E-2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>6.1103728733517588</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>1.5275932183379397</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="4"/>
+        <v>254.40047343763285</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="5"/>
+        <v>1017.6018937505314</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="6"/>
+        <v>50.880094687526572</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>5.7371473469387757</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>0.13115583061224487</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>5.7386463153247407</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>1.4346615788311852</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="4"/>
+        <v>233.94630531084411</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="5"/>
+        <v>935.78522124337644</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="6"/>
+        <v>38.991050885140687</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>5.2931121428571437</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>0.1780739214285714</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>5.2961067283764862</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>1.3240266820941216</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="4"/>
+        <v>210.43649651945179</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="5"/>
+        <v>841.74598607780717</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="6"/>
+        <v>30.062356645635969</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>4.7775836734693886</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>0.23215166530612241</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>4.7832206882712054</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>1.1958051720678013</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="4"/>
+        <v>184.33297367540058</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="5"/>
+        <v>737.33189470160232</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="6"/>
+        <v>23.041621709425073</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>4.1905619387755113</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>0.29338906224489791</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>4.2008197419740485</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>1.0502049354935121</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="4"/>
+        <v>156.17993273748374</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="5"/>
+        <v>624.71973094993496</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="6"/>
+        <v>17.353325859720414</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>3.5320469387755105</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>0.36178611224489798</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>3.5505273930399035</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>0.88763184825997588</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="4"/>
+        <v>126.61552826528921</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="5"/>
+        <v>506.46211306115686</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="6"/>
+        <v>12.661552826528922</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>2.8020386734693883</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>0.43734281530612235</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>2.8359635868110109</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="3"/>
+        <v>0.70899089670275273</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="4"/>
+        <v>96.404847693540518</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="5"/>
+        <v>385.61939077416207</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="6"/>
+        <v>8.7640770630491378</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>2.0005371428571435</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>0.52005917142857139</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>2.0670293664430592</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="3"/>
+        <v>0.51675734161076481</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="4"/>
+        <v>66.557209098428785</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="5"/>
+        <v>266.22883639371514</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="6"/>
+        <v>5.5464340915357324</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>1.1275423469387755</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>0.60993518061224483</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>1.2819409770690278</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="3"/>
+        <v>0.32048524426725694</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="4"/>
+        <v>38.929372093844449</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="5"/>
+        <v>155.7174883753778</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="6"/>
+        <v>2.9945670841418806</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>0.18305428571428628</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>0.70697084285714262</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>0.73028531696077947</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>0.18257132924019487</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="4"/>
+        <v>21.23690756686598</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="5"/>
+        <v>84.947630267463921</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="6"/>
+        <v>1.5169219690618558</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>0.81116615816326509</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>0.81116615816326509</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>0.20279153954081627</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="4"/>
+        <v>23.74203515326284</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="5"/>
+        <v>94.968140613051361</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="6"/>
+        <v>1.582802343550856</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>0.92252112653061213</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>0.92252112653061213</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="3"/>
+        <v>0.23063028163265303</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="4"/>
+        <v>27.24098964994322</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="5"/>
+        <v>108.96395859977288</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="6"/>
+        <v>1.7025618531214513</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>1.0410357479591834</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>1.0410357479591834</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>0.26025893698979585</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="4"/>
+        <v>31.028480775866065</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="5"/>
+        <v>124.11392310346426</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="6"/>
+        <v>1.8252047515215333</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>1.1667100224489795</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>1.1667100224489795</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="3"/>
+        <v>0.29167750561224487</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="4"/>
+        <v>35.116388213019121</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="5"/>
+        <v>140.46555285207648</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="6"/>
+        <v>1.95091045627884</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>1.2995439499999999</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>1.2995439499999999</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="3"/>
+        <v>0.32488598749999997</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="4"/>
+        <v>39.517309313501073</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="5"/>
+        <v>158.06923725400429</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="6"/>
+        <v>2.079858384921109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>1.4395375306122449</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>1.4395375306122449</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="3"/>
+        <v>0.35988438265306122</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="4"/>
+        <v>44.244559099521553</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="5"/>
+        <v>176.97823639808621</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="6"/>
+        <v>2.2122279549760777</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>1.586690764285714</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>1.586690764285714</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="3"/>
+        <v>0.3966726910714285</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="4"/>
+        <v>49.31217026340115</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="5"/>
+        <v>197.2486810536046</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="6"/>
+        <v>2.3481985839714832</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <f>IF(6.9-(0.350317*A23*A23-0.202576*A23)/9.8&gt;0, 6.9-(0.350317*A23*A23-0.202576*A23)/9.8, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <f>(0.0350823*A23*A23+0.00372739*A23)/9.8</f>
+        <v>1.7410036510204079</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>1.7410036510204079</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="3"/>
+        <v>0.43525091275510197</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="4"/>
+        <v>54.7348931675714</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="5"/>
+        <v>218.9395726702856</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="6"/>
+        <v>2.4879496894350637</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <f>IF(6.9-(0.350317*A24*A24-0.202576*A24)/9.8&gt;0, 6.9-(0.350317*A24*A24-0.202576*A24)/9.8, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <f>(0.0350823*A24*A24+0.00372739*A24)/9.8</f>
+        <v>1.9024761908163261</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>1.9024761908163261</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="3"/>
+        <v>0.47561904770408153</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="4"/>
+        <v>60.528195844574803</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="5"/>
+        <v>242.11278337829921</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="6"/>
+        <v>2.6316606888945566</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <f>IF(6.9-(0.350317*A25*A25-0.202576*A25)/9.8&gt;0, 6.9-(0.350317*A25*A25-0.202576*A25)/9.8, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <f>(0.0350823*A25*A25+0.00372739*A25)/9.8</f>
+        <v>2.0711083836734692</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>2.0711083836734692</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="3"/>
+        <v>0.51777709591836729</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="4"/>
+        <v>66.708263997064805</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="5"/>
+        <v>266.83305598825922</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="6"/>
+        <v>2.7795109998777003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <f t="shared" ref="B26:B31" si="7">IF(6.9-(0.350317*A26*A26-0.202576*A26)/9.8&gt;0, 6.9-(0.350317*A26*A26-0.202576*A26)/9.8, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ref="C26:C31" si="8">(0.0350823*A26*A26+0.00372739*A26)/9.8</f>
+        <v>2.2469002295918363</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>2.2469002295918363</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="3"/>
+        <v>0.56172505739795908</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="4"/>
+        <v>73.292000997805772</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="5"/>
+        <v>293.16800399122309</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="6"/>
+        <v>2.9316800399122309</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="8"/>
+        <v>2.4298517285714283</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>2.4298517285714283</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="3"/>
+        <v>0.60746293214285707</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="4"/>
+        <v>80.29702788967306</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="5"/>
+        <v>321.18811155869224</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="6"/>
+        <v>3.0883472265258871</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="8"/>
+        <v>2.6199628806122446</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="2"/>
+        <v>2.6199628806122446</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="3"/>
+        <v>0.65499072015306115</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="4"/>
+        <v>87.741683385652948</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="5"/>
+        <v>350.96673354261179</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="6"/>
+        <v>3.2496919772464055</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="8"/>
+        <v>2.8172336857142848</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>2.8172336857142848</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="3"/>
+        <v>0.7043084214285712</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="4"/>
+        <v>95.645023868842657</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="5"/>
+        <v>382.58009547537063</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="6"/>
+        <v>3.4158937096015234</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="8"/>
+        <v>3.0216641438775502</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>3.0216641438775502</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="3"/>
+        <v>0.75541603596938756</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="4"/>
+        <v>104.02682339245044</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="5"/>
+        <v>416.10729356980175</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="6"/>
+        <v>3.5871318411189805</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="8"/>
+        <v>3.23325425510204</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="2"/>
+        <v>3.23325425510204</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="3"/>
+        <v>0.80831356377551</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="4"/>
+        <v>112.90757367979539</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="5"/>
+        <v>451.63029471918156</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="6"/>
+        <v>3.763585789326513</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Calculate cruise speed without payload
</commit_message>
<xml_diff>
--- a/Power & Propulsion System/Power Consumption.xlsx
+++ b/Power & Propulsion System/Power Consumption.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\Videos\UAS_Challenge\Power &amp; Propulsion System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244BC670-9B55-4402-89F9-DE6F0545D541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5BFEEE-8790-4938-A3B6-CA1784A9E3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power &amp; Thrust Data" sheetId="3" r:id="rId1"/>
     <sheet name="Drag &amp; Lift Data" sheetId="2" r:id="rId2"/>
     <sheet name="Cruise Speed (Loaded)" sheetId="4" r:id="rId3"/>
+    <sheet name="Cruise Speed (Empty)" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>Propeller</t>
   </si>
@@ -2179,18 +2180,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:B12"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="A2:A23"/>
+    <mergeCell ref="A24:A45"/>
+    <mergeCell ref="B24:B34"/>
+    <mergeCell ref="B35:B45"/>
     <mergeCell ref="A79:A80"/>
     <mergeCell ref="B79:B80"/>
     <mergeCell ref="B46:B56"/>
     <mergeCell ref="B57:B67"/>
     <mergeCell ref="B68:B78"/>
     <mergeCell ref="A46:A78"/>
-    <mergeCell ref="B2:B12"/>
-    <mergeCell ref="B13:B23"/>
-    <mergeCell ref="A2:A23"/>
-    <mergeCell ref="A24:A45"/>
-    <mergeCell ref="B24:B34"/>
-    <mergeCell ref="B35:B45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2334,7 +2335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC55B06D-1837-44EB-A9AC-10712F976789}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -3368,4 +3369,1043 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB64D9D4-5BCC-49AE-83E3-4307C103F2F6}">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="17.7265625" customWidth="1"/>
+    <col min="4" max="4" width="15.6328125" customWidth="1"/>
+    <col min="5" max="6" width="18.54296875" customWidth="1"/>
+    <col min="7" max="7" width="13.6328125" customWidth="1"/>
+    <col min="8" max="8" width="16.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>IF(3.5-(0.350317*A2*A2-0.202576*A2)/9.8&gt;0, 3.5-(0.350317*A2*A2-0.202576*A2)/9.8, 0)</f>
+        <v>3.4849243877551022</v>
+      </c>
+      <c r="C2">
+        <f>(0.0350823*A2*A2+0.00372739*A2)/9.8</f>
+        <v>3.960172448979591E-3</v>
+      </c>
+      <c r="D2">
+        <f>SQRT(C2*C2+B2*B2)</f>
+        <v>3.4849266378700281</v>
+      </c>
+      <c r="E2">
+        <f>D2/4</f>
+        <v>0.87123165946750702</v>
+      </c>
+      <c r="F2">
+        <f>1000000*0.0000373344395*E2*E2+ 1000*0.109504955*E2</f>
+        <v>123.74268852752219</v>
+      </c>
+      <c r="G2">
+        <f>F2*4</f>
+        <v>494.97075411008876</v>
+      </c>
+      <c r="H2">
+        <f>F2/A2</f>
+        <v>123.74268852752219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B31" si="0">IF(3.5-(0.350317*A3*A3-0.202576*A3)/9.8&gt;0, 3.5-(0.350317*A3*A3-0.202576*A3)/9.8, 0)</f>
+        <v>3.3983555102040817</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C22" si="1">(0.0350823*A3*A3+0.00372739*A3)/9.8</f>
+        <v>1.5079997959183671E-2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D31" si="2">SQRT(C3*C3+B3*B3)</f>
+        <v>3.398388968330861</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E31" si="3">D3/4</f>
+        <v>0.84959724208271525</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F31" si="4">1000000*0.0000373344395*E3*E3+ 1000*0.109504955*E3</f>
+        <v>119.98368389744513</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G31" si="5">F3*4</f>
+        <v>479.93473558978053</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H31" si="6">F3/A3</f>
+        <v>59.991841948722566</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>3.240293367346939</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>3.3359476530612241E-2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="2"/>
+        <v>3.2404650840808271</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="3"/>
+        <v>0.81011627102020678</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="4"/>
+        <v>113.21390434316658</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="5"/>
+        <v>452.8556173726663</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="6"/>
+        <v>37.737968114388856</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>3.0107379591836736</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>5.8798608163265292E-2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>3.0113120620738409</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="3"/>
+        <v>0.75282801551846024</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="4"/>
+        <v>103.59769233084975</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="5"/>
+        <v>414.39076932339901</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="6"/>
+        <v>25.899423082712438</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>2.709689285714286</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>9.1397392857142851E-2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>2.7112302573805644</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>0.67780756434514111</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="4"/>
+        <v>91.375590550704132</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="5"/>
+        <v>365.50236220281653</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="6"/>
+        <v>18.275118110140827</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>2.3371473469387753</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>0.13115583061224487</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>2.3408245498555726</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>0.58520613746389316</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="4"/>
+        <v>76.8687562442434</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="5"/>
+        <v>307.4750249769736</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="6"/>
+        <v>12.811459374040567</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>1.8931121428571429</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>0.1780739214285714</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>1.9014688813983027</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>0.47536722034957568</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="4"/>
+        <v>60.49167848724953</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="5"/>
+        <v>241.96671394899812</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="6"/>
+        <v>8.6416683553213609</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>1.3775836734693883</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>0.23215166530612241</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>1.3970079359523409</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>0.34925198398808521</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="4"/>
+        <v>42.798763787709234</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="5"/>
+        <v>171.19505515083694</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="6"/>
+        <v>5.3498454734636542</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>0.79056193877551051</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>0.29338906224489791</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>0.84324689201053948</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>0.21081172300263487</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="4"/>
+        <v>24.744129816072579</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="5"/>
+        <v>98.976519264290317</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="6"/>
+        <v>2.7493477573413978</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>0.1320469387755101</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>0.36178611224489798</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>0.38513060778554231</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>9.6282651946385578E-2</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="4"/>
+        <v>10.889530755011682</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="5"/>
+        <v>43.558123020046729</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="6"/>
+        <v>1.0889530755011683</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>0.43734281530612235</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>0.43734281530612235</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="3"/>
+        <v>0.10933570382653059</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="4"/>
+        <v>12.419108273094528</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="5"/>
+        <v>49.676433092378112</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="6"/>
+        <v>1.1290098430085935</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>0.52005917142857139</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>0.52005917142857139</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="3"/>
+        <v>0.13001479285714285</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="4"/>
+        <v>14.8683596704634</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="5"/>
+        <v>59.473438681853601</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="6"/>
+        <v>1.2390299725386167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>0.60993518061224483</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>0.60993518061224483</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="3"/>
+        <v>0.15248379515306121</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="4"/>
+        <v>17.565805670233296</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="5"/>
+        <v>70.263222680933183</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="6"/>
+        <v>1.3512158207871765</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>0.70697084285714262</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>0.70697084285714262</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>0.17674271071428566</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="4"/>
+        <v>20.520455273948137</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="5"/>
+        <v>82.081821095792549</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="6"/>
+        <v>1.4657468052820097</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>0.81116615816326509</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>0.81116615816326509</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>0.20279153954081627</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="4"/>
+        <v>23.74203515326284</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="5"/>
+        <v>94.968140613051361</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="6"/>
+        <v>1.582802343550856</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>0.92252112653061213</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>0.92252112653061213</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="3"/>
+        <v>0.23063028163265303</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="4"/>
+        <v>27.24098964994322</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="5"/>
+        <v>108.96395859977288</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="6"/>
+        <v>1.7025618531214513</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>1.0410357479591834</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>1.0410357479591834</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>0.26025893698979585</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="4"/>
+        <v>31.028480775866065</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="5"/>
+        <v>124.11392310346426</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="6"/>
+        <v>1.8252047515215333</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>1.1667100224489795</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>1.1667100224489795</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="3"/>
+        <v>0.29167750561224487</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="4"/>
+        <v>35.116388213019121</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="5"/>
+        <v>140.46555285207648</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="6"/>
+        <v>1.95091045627884</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>1.2995439499999999</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>1.2995439499999999</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="3"/>
+        <v>0.32488598749999997</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="4"/>
+        <v>39.517309313501073</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="5"/>
+        <v>158.06923725400429</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="6"/>
+        <v>2.079858384921109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>1.4395375306122449</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>1.4395375306122449</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="3"/>
+        <v>0.35988438265306122</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="4"/>
+        <v>44.244559099521553</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="5"/>
+        <v>176.97823639808621</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="6"/>
+        <v>2.2122279549760777</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>1.586690764285714</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>1.586690764285714</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="3"/>
+        <v>0.3966726910714285</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="4"/>
+        <v>49.31217026340115</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="5"/>
+        <v>197.2486810536046</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="6"/>
+        <v>2.3481985839714832</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <f>(0.0350823*A23*A23+0.00372739*A23)/9.8</f>
+        <v>1.7410036510204079</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>1.7410036510204079</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="3"/>
+        <v>0.43525091275510197</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="4"/>
+        <v>54.7348931675714</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="5"/>
+        <v>218.9395726702856</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="6"/>
+        <v>2.4879496894350637</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <f>(0.0350823*A24*A24+0.00372739*A24)/9.8</f>
+        <v>1.9024761908163261</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>1.9024761908163261</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="3"/>
+        <v>0.47561904770408153</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="4"/>
+        <v>60.528195844574803</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="5"/>
+        <v>242.11278337829921</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="6"/>
+        <v>2.6316606888945566</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <f>(0.0350823*A25*A25+0.00372739*A25)/9.8</f>
+        <v>2.0711083836734692</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>2.0711083836734692</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="3"/>
+        <v>0.51777709591836729</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="4"/>
+        <v>66.708263997064805</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="5"/>
+        <v>266.83305598825922</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="6"/>
+        <v>2.7795109998777003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ref="C26:C31" si="7">(0.0350823*A26*A26+0.00372739*A26)/9.8</f>
+        <v>2.2469002295918363</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>2.2469002295918363</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="3"/>
+        <v>0.56172505739795908</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="4"/>
+        <v>73.292000997805772</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="5"/>
+        <v>293.16800399122309</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="6"/>
+        <v>2.9316800399122309</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="7"/>
+        <v>2.4298517285714283</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>2.4298517285714283</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="3"/>
+        <v>0.60746293214285707</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="4"/>
+        <v>80.29702788967306</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="5"/>
+        <v>321.18811155869224</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="6"/>
+        <v>3.0883472265258871</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="7"/>
+        <v>2.6199628806122446</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="2"/>
+        <v>2.6199628806122446</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="3"/>
+        <v>0.65499072015306115</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="4"/>
+        <v>87.741683385652948</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="5"/>
+        <v>350.96673354261179</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="6"/>
+        <v>3.2496919772464055</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="7"/>
+        <v>2.8172336857142848</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>2.8172336857142848</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="3"/>
+        <v>0.7043084214285712</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="4"/>
+        <v>95.645023868842657</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="5"/>
+        <v>382.58009547537063</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="6"/>
+        <v>3.4158937096015234</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="7"/>
+        <v>3.0216641438775502</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>3.0216641438775502</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="3"/>
+        <v>0.75541603596938756</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="4"/>
+        <v>104.02682339245044</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="5"/>
+        <v>416.10729356980175</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="6"/>
+        <v>3.5871318411189805</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="7"/>
+        <v>3.23325425510204</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="2"/>
+        <v>3.23325425510204</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="3"/>
+        <v>0.80831356377551</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="4"/>
+        <v>112.90757367979539</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="5"/>
+        <v>451.63029471918156</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="6"/>
+        <v>3.763585789326513</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Calculate mission power & energy consumed in cruise
</commit_message>
<xml_diff>
--- a/Power & Propulsion System/Power Consumption.xlsx
+++ b/Power & Propulsion System/Power Consumption.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\Videos\UAS_Challenge\Power &amp; Propulsion System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5BFEEE-8790-4938-A3B6-CA1784A9E3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3717961D-DEBA-44ED-A83C-DE9DBB173B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power &amp; Thrust Data" sheetId="3" r:id="rId1"/>
     <sheet name="Drag &amp; Lift Data" sheetId="2" r:id="rId2"/>
     <sheet name="Cruise Speed (Loaded)" sheetId="4" r:id="rId3"/>
     <sheet name="Cruise Speed (Empty)" sheetId="5" r:id="rId4"/>
+    <sheet name="Flight Data" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>Propeller</t>
   </si>
@@ -127,6 +128,42 @@
   </si>
   <si>
     <t>Cruise Efficiency</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Time (s)</t>
+  </si>
+  <si>
+    <t>Average Vertical Thrust (kgf)</t>
+  </si>
+  <si>
+    <t>Average Horizontal Thrust (kgf)</t>
+  </si>
+  <si>
+    <t>Average Total Thrust (kgf)</t>
+  </si>
+  <si>
+    <t>Average Power Consumed (W)</t>
+  </si>
+  <si>
+    <t>Total Energy Consumed (Wh)</t>
+  </si>
+  <si>
+    <t>Take-off</t>
+  </si>
+  <si>
+    <t>Cruise to SZ</t>
+  </si>
+  <si>
+    <t>Spray Zone</t>
+  </si>
+  <si>
+    <t>Cruise to Landing</t>
+  </si>
+  <si>
+    <t>Landing</t>
   </si>
 </sst>
 </file>
@@ -2180,18 +2217,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="B46:B56"/>
+    <mergeCell ref="B57:B67"/>
+    <mergeCell ref="B68:B78"/>
+    <mergeCell ref="A46:A78"/>
     <mergeCell ref="B2:B12"/>
     <mergeCell ref="B13:B23"/>
     <mergeCell ref="A2:A23"/>
     <mergeCell ref="A24:A45"/>
     <mergeCell ref="B24:B34"/>
     <mergeCell ref="B35:B45"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="B46:B56"/>
-    <mergeCell ref="B57:B67"/>
-    <mergeCell ref="B68:B78"/>
-    <mergeCell ref="A46:A78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3375,7 +3412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB64D9D4-5BCC-49AE-83E3-4307C103F2F6}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -4408,4 +4445,140 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893ADDC9-523C-47B1-8967-17603EEDB938}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.90625" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" customWidth="1"/>
+    <col min="4" max="4" width="28.26953125" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="27.54296875" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2">
+        <f>SQRT(D2*D2+C2*C2)</f>
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f>B2*F2/3600</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>134</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>3.23</v>
+      </c>
+      <c r="E3">
+        <f>SQRT(D3*D3+C3*C3)</f>
+        <v>3.23</v>
+      </c>
+      <c r="F3">
+        <v>451</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G6" si="0">B3*F3/3600</f>
+        <v>16.787222222222223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E6" si="1">SQRT(D4*D4+C4*C4)</f>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>3.23</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>3.23</v>
+      </c>
+      <c r="F5">
+        <v>451</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>2.1297222222222221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified Power Consumption Calculations
</commit_message>
<xml_diff>
--- a/Power & Propulsion System/Power Consumption.xlsx
+++ b/Power & Propulsion System/Power Consumption.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\Videos\UAS_Challenge\Power &amp; Propulsion System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17157551-241B-4668-AF78-23B31047DCC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD0D438-C852-4280-B0B2-46B816CCAB6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="806" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="806" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Motors" sheetId="3" r:id="rId1"/>
@@ -463,6 +463,7 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -472,7 +473,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -807,10 +807,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C2">
@@ -832,8 +832,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
       <c r="C3">
         <v>47.39</v>
       </c>
@@ -853,8 +853,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
       <c r="C4">
         <v>47.36</v>
       </c>
@@ -874,8 +874,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
       <c r="C5">
         <v>47.34</v>
       </c>
@@ -895,8 +895,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
       <c r="C6">
         <v>47.31</v>
       </c>
@@ -916,8 +916,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
       <c r="C7">
         <v>47.28</v>
       </c>
@@ -937,8 +937,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
       <c r="C8">
         <v>47.24</v>
       </c>
@@ -958,8 +958,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
       <c r="C9">
         <v>47.21</v>
       </c>
@@ -979,8 +979,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
       <c r="C10">
         <v>47.17</v>
       </c>
@@ -1000,8 +1000,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
       <c r="C11">
         <v>47.08</v>
       </c>
@@ -1021,8 +1021,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
       <c r="C12">
         <v>47.03</v>
       </c>
@@ -1042,8 +1042,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="1" t="s">
+      <c r="A13" s="3"/>
+      <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C13">
@@ -1065,8 +1065,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
       <c r="C14">
         <v>47.37</v>
       </c>
@@ -1086,8 +1086,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
       <c r="C15">
         <v>47.34</v>
       </c>
@@ -1107,8 +1107,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
       <c r="C16">
         <v>47.3</v>
       </c>
@@ -1128,8 +1128,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
       <c r="C17">
         <v>47.27</v>
       </c>
@@ -1149,8 +1149,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
       <c r="C18">
         <v>47.23</v>
       </c>
@@ -1170,8 +1170,8 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
       <c r="C19">
         <v>47.19</v>
       </c>
@@ -1191,8 +1191,8 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
       <c r="C20">
         <v>47.15</v>
       </c>
@@ -1212,8 +1212,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
       <c r="C21">
         <v>47.1</v>
       </c>
@@ -1233,8 +1233,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
       <c r="C22">
         <v>46.99</v>
       </c>
@@ -1254,8 +1254,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
       <c r="C23">
         <v>46.94</v>
       </c>
@@ -1275,10 +1275,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C24">
@@ -1300,8 +1300,8 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
       <c r="C25">
         <v>23.43</v>
       </c>
@@ -1321,8 +1321,8 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
       <c r="C26">
         <v>23.38</v>
       </c>
@@ -1342,8 +1342,8 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
       <c r="C27">
         <v>23.33</v>
       </c>
@@ -1363,8 +1363,8 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
       <c r="C28">
         <v>23.27</v>
       </c>
@@ -1384,8 +1384,8 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
       <c r="C29">
         <v>23.21</v>
       </c>
@@ -1405,8 +1405,8 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
       <c r="C30">
         <v>23.15</v>
       </c>
@@ -1426,8 +1426,8 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
       <c r="C31">
         <v>23.08</v>
       </c>
@@ -1447,8 +1447,8 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
       <c r="C32">
         <v>23</v>
       </c>
@@ -1468,8 +1468,8 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
       <c r="C33">
         <v>22.82</v>
       </c>
@@ -1489,8 +1489,8 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
       <c r="C34">
         <v>22.72</v>
       </c>
@@ -1510,8 +1510,8 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="2"/>
-      <c r="B35" s="1" t="s">
+      <c r="A35" s="3"/>
+      <c r="B35" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C35">
@@ -1533,8 +1533,8 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
       <c r="C36">
         <v>23.39</v>
       </c>
@@ -1554,8 +1554,8 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
       <c r="C37">
         <v>23.33</v>
       </c>
@@ -1575,8 +1575,8 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
       <c r="C38">
         <v>23.26</v>
       </c>
@@ -1596,8 +1596,8 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
       <c r="C39">
         <v>23.19</v>
       </c>
@@ -1617,8 +1617,8 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
       <c r="C40">
         <v>23.11</v>
       </c>
@@ -1638,8 +1638,8 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
       <c r="C41">
         <v>23.04</v>
       </c>
@@ -1659,8 +1659,8 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
       <c r="C42">
         <v>22.95</v>
       </c>
@@ -1680,8 +1680,8 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
       <c r="C43">
         <v>22.86</v>
       </c>
@@ -1701,8 +1701,8 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
       <c r="C44">
         <v>22.63</v>
       </c>
@@ -1722,8 +1722,8 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
       <c r="C45">
         <v>22.51</v>
       </c>
@@ -1743,10 +1743,10 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C46">
@@ -1768,8 +1768,8 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" s="1"/>
-      <c r="B47" s="2"/>
+      <c r="A47" s="2"/>
+      <c r="B47" s="3"/>
       <c r="C47">
         <v>23.44</v>
       </c>
@@ -1789,8 +1789,8 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="1"/>
-      <c r="B48" s="2"/>
+      <c r="A48" s="2"/>
+      <c r="B48" s="3"/>
       <c r="C48">
         <v>23.4</v>
       </c>
@@ -1810,8 +1810,8 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A49" s="1"/>
-      <c r="B49" s="2"/>
+      <c r="A49" s="2"/>
+      <c r="B49" s="3"/>
       <c r="C49">
         <v>23.35</v>
       </c>
@@ -1831,8 +1831,8 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A50" s="1"/>
-      <c r="B50" s="2"/>
+      <c r="A50" s="2"/>
+      <c r="B50" s="3"/>
       <c r="C50">
         <v>23.3</v>
       </c>
@@ -1852,8 +1852,8 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A51" s="1"/>
-      <c r="B51" s="2"/>
+      <c r="A51" s="2"/>
+      <c r="B51" s="3"/>
       <c r="C51">
         <v>23.25</v>
       </c>
@@ -1873,8 +1873,8 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A52" s="1"/>
-      <c r="B52" s="2"/>
+      <c r="A52" s="2"/>
+      <c r="B52" s="3"/>
       <c r="C52">
         <v>23.19</v>
       </c>
@@ -1894,8 +1894,8 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" s="1"/>
-      <c r="B53" s="2"/>
+      <c r="A53" s="2"/>
+      <c r="B53" s="3"/>
       <c r="C53">
         <v>23.13</v>
       </c>
@@ -1915,8 +1915,8 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A54" s="1"/>
-      <c r="B54" s="2"/>
+      <c r="A54" s="2"/>
+      <c r="B54" s="3"/>
       <c r="C54">
         <v>23.06</v>
       </c>
@@ -1936,8 +1936,8 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A55" s="1"/>
-      <c r="B55" s="2"/>
+      <c r="A55" s="2"/>
+      <c r="B55" s="3"/>
       <c r="C55">
         <v>22.9</v>
       </c>
@@ -1957,8 +1957,8 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A56" s="1"/>
-      <c r="B56" s="2"/>
+      <c r="A56" s="2"/>
+      <c r="B56" s="3"/>
       <c r="C56">
         <v>22.81</v>
       </c>
@@ -1978,8 +1978,8 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1" t="s">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C57">
@@ -2001,8 +2001,8 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A58" s="1"/>
-      <c r="B58" s="2"/>
+      <c r="A58" s="2"/>
+      <c r="B58" s="3"/>
       <c r="C58">
         <v>23.41</v>
       </c>
@@ -2022,8 +2022,8 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A59" s="1"/>
-      <c r="B59" s="2"/>
+      <c r="A59" s="2"/>
+      <c r="B59" s="3"/>
       <c r="C59">
         <v>23.36</v>
       </c>
@@ -2043,8 +2043,8 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A60" s="1"/>
-      <c r="B60" s="2"/>
+      <c r="A60" s="2"/>
+      <c r="B60" s="3"/>
       <c r="C60">
         <v>23.31</v>
       </c>
@@ -2064,8 +2064,8 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A61" s="1"/>
-      <c r="B61" s="2"/>
+      <c r="A61" s="2"/>
+      <c r="B61" s="3"/>
       <c r="C61">
         <v>23.25</v>
       </c>
@@ -2085,8 +2085,8 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A62" s="1"/>
-      <c r="B62" s="2"/>
+      <c r="A62" s="2"/>
+      <c r="B62" s="3"/>
       <c r="C62">
         <v>23.19</v>
       </c>
@@ -2106,8 +2106,8 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A63" s="1"/>
-      <c r="B63" s="2"/>
+      <c r="A63" s="2"/>
+      <c r="B63" s="3"/>
       <c r="C63">
         <v>23.13</v>
       </c>
@@ -2127,8 +2127,8 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A64" s="1"/>
-      <c r="B64" s="2"/>
+      <c r="A64" s="2"/>
+      <c r="B64" s="3"/>
       <c r="C64">
         <v>23.05</v>
       </c>
@@ -2148,8 +2148,8 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A65" s="1"/>
-      <c r="B65" s="2"/>
+      <c r="A65" s="2"/>
+      <c r="B65" s="3"/>
       <c r="C65">
         <v>22.96</v>
       </c>
@@ -2169,8 +2169,8 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A66" s="1"/>
-      <c r="B66" s="2"/>
+      <c r="A66" s="2"/>
+      <c r="B66" s="3"/>
       <c r="C66">
         <v>22.77</v>
       </c>
@@ -2190,8 +2190,8 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A67" s="1"/>
-      <c r="B67" s="2"/>
+      <c r="A67" s="2"/>
+      <c r="B67" s="3"/>
       <c r="C67">
         <v>22.67</v>
       </c>
@@ -2211,8 +2211,8 @@
       </c>
     </row>
     <row r="68" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1" t="s">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C68">
@@ -2234,8 +2234,8 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A69" s="1"/>
-      <c r="B69" s="2"/>
+      <c r="A69" s="2"/>
+      <c r="B69" s="3"/>
       <c r="C69">
         <v>23.39</v>
       </c>
@@ -2255,8 +2255,8 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A70" s="1"/>
-      <c r="B70" s="2"/>
+      <c r="A70" s="2"/>
+      <c r="B70" s="3"/>
       <c r="C70">
         <v>23.33</v>
       </c>
@@ -2276,8 +2276,8 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A71" s="1"/>
-      <c r="B71" s="2"/>
+      <c r="A71" s="2"/>
+      <c r="B71" s="3"/>
       <c r="C71">
         <v>23.26</v>
       </c>
@@ -2297,8 +2297,8 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A72" s="1"/>
-      <c r="B72" s="2"/>
+      <c r="A72" s="2"/>
+      <c r="B72" s="3"/>
       <c r="C72">
         <v>23.2</v>
       </c>
@@ -2318,8 +2318,8 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A73" s="1"/>
-      <c r="B73" s="2"/>
+      <c r="A73" s="2"/>
+      <c r="B73" s="3"/>
       <c r="C73">
         <v>23.13</v>
       </c>
@@ -2339,8 +2339,8 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A74" s="1"/>
-      <c r="B74" s="2"/>
+      <c r="A74" s="2"/>
+      <c r="B74" s="3"/>
       <c r="C74">
         <v>23.05</v>
       </c>
@@ -2360,8 +2360,8 @@
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A75" s="1"/>
-      <c r="B75" s="2"/>
+      <c r="A75" s="2"/>
+      <c r="B75" s="3"/>
       <c r="C75">
         <v>22.97</v>
       </c>
@@ -2381,8 +2381,8 @@
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A76" s="1"/>
-      <c r="B76" s="2"/>
+      <c r="A76" s="2"/>
+      <c r="B76" s="3"/>
       <c r="C76">
         <v>22.87</v>
       </c>
@@ -2402,8 +2402,8 @@
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A77" s="1"/>
-      <c r="B77" s="2"/>
+      <c r="A77" s="2"/>
+      <c r="B77" s="3"/>
       <c r="C77">
         <v>22.65</v>
       </c>
@@ -2423,8 +2423,8 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A78" s="1"/>
-      <c r="B78" s="2"/>
+      <c r="A78" s="2"/>
+      <c r="B78" s="3"/>
       <c r="C78">
         <v>22.53</v>
       </c>
@@ -2444,10 +2444,10 @@
       </c>
     </row>
     <row r="79" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="1" t="s">
+      <c r="A79" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B79" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C79">
@@ -2469,8 +2469,8 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A80" s="1"/>
-      <c r="B80" s="2"/>
+      <c r="A80" s="2"/>
+      <c r="B80" s="3"/>
       <c r="C80">
         <v>15.43</v>
       </c>
@@ -2490,8 +2490,8 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A81" s="1"/>
-      <c r="B81" s="2"/>
+      <c r="A81" s="2"/>
+      <c r="B81" s="3"/>
       <c r="C81">
         <v>15.21</v>
       </c>
@@ -2511,8 +2511,8 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A82" s="1"/>
-      <c r="B82" s="2"/>
+      <c r="A82" s="2"/>
+      <c r="B82" s="3"/>
       <c r="C82">
         <v>14.93</v>
       </c>
@@ -2532,8 +2532,8 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A83" s="1"/>
-      <c r="B83" s="2"/>
+      <c r="A83" s="2"/>
+      <c r="B83" s="3"/>
       <c r="C83">
         <v>14.68</v>
       </c>
@@ -2553,8 +2553,8 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A84" s="1"/>
-      <c r="B84" s="2"/>
+      <c r="A84" s="2"/>
+      <c r="B84" s="3"/>
       <c r="C84">
         <v>14.47</v>
       </c>
@@ -2575,18 +2575,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:B12"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="A2:A23"/>
+    <mergeCell ref="A24:A45"/>
+    <mergeCell ref="B24:B34"/>
+    <mergeCell ref="B35:B45"/>
     <mergeCell ref="B46:B56"/>
     <mergeCell ref="B57:B67"/>
     <mergeCell ref="B68:B78"/>
     <mergeCell ref="A46:A78"/>
     <mergeCell ref="A79:A84"/>
     <mergeCell ref="B79:B84"/>
-    <mergeCell ref="B2:B12"/>
-    <mergeCell ref="B13:B23"/>
-    <mergeCell ref="A2:A23"/>
-    <mergeCell ref="A24:A45"/>
-    <mergeCell ref="B24:B34"/>
-    <mergeCell ref="B35:B45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2594,10 +2594,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DCE7B62-FB69-4347-8AA6-5823B55756E6}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2656,11 +2656,11 @@
         <v>0.56971285000000005</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D6" si="0">0.350317*A3*A3-0.202576*A3</f>
+        <f t="shared" ref="D3:D20" si="0">0.350317*A3*A3-0.202576*A3</f>
         <v>4.7947679999999995</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E6" si="1">0.0350823*A3*A3+0.00372739*A3</f>
+        <f t="shared" ref="E3:E20" si="1">0.0350823*A3*A3+0.00372739*A3</f>
         <v>0.57622635999999994</v>
       </c>
     </row>
@@ -2719,6 +2719,188 @@
       <c r="E6">
         <f t="shared" si="1"/>
         <v>9.0407070399999991</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>136.07527999999999</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>14.1074678</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>196.92076799999998</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>20.29686216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>28</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>268.97640000000001</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>27.608890119999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>32</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>352.24217599999997</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>36.04355168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>36</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>446.718096</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>45.600846840000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>40</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>552.40416000000005</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>56.280775600000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>44</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>669.30036799999993</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>68.083337959999994</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>48</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>797.40671999999995</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>81.008533919999991</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>52</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>936.72321600000009</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>95.056363480000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>56</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>1087.2498559999999</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>110.22682663999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>60</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>1248.9866399999999</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>126.51992339999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>64</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>1421.9335679999999</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>143.93565375999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>68</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>1606.0906400000001</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>162.47401771999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>72</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>1801.457856</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>182.13501528</v>
       </c>
     </row>
   </sheetData>
@@ -2730,7 +2912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC55B06D-1837-44EB-A9AC-10712F976789}">
   <dimension ref="A1:K306"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
     </sheetView>
@@ -43314,7 +43496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893ADDC9-523C-47B1-8967-17603EEDB938}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -43327,24 +43509,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -43371,7 +43553,7 @@
         <v>2100</v>
       </c>
       <c r="D5">
-        <f>B5*C5/3600</f>
+        <f t="shared" ref="D5:D13" si="0">B5*C5/3600</f>
         <v>1.75</v>
       </c>
     </row>
@@ -43386,7 +43568,7 @@
         <v>2560</v>
       </c>
       <c r="D6">
-        <f>B6*C6/3600</f>
+        <f t="shared" si="0"/>
         <v>1.0666666666666667</v>
       </c>
     </row>
@@ -43401,7 +43583,7 @@
         <v>85</v>
       </c>
       <c r="D7">
-        <f>B7*C7/3600</f>
+        <f t="shared" si="0"/>
         <v>6.6583333333333332</v>
       </c>
     </row>
@@ -43416,7 +43598,7 @@
         <v>2560</v>
       </c>
       <c r="D8">
-        <f>B8*C8/3600</f>
+        <f t="shared" si="0"/>
         <v>1.0666666666666667</v>
       </c>
     </row>
@@ -43431,7 +43613,7 @@
         <v>488</v>
       </c>
       <c r="D9">
-        <f>B9*C9/3600</f>
+        <f t="shared" si="0"/>
         <v>28.466666666666665</v>
       </c>
     </row>
@@ -43446,7 +43628,7 @@
         <v>2560</v>
       </c>
       <c r="D10">
-        <f>B10*C10/3600</f>
+        <f t="shared" si="0"/>
         <v>1.0666666666666667</v>
       </c>
     </row>
@@ -43461,7 +43643,7 @@
         <v>47.833199999999998</v>
       </c>
       <c r="D11">
-        <f>B11*C11/3600</f>
+        <f t="shared" si="0"/>
         <v>0.62050290000000008</v>
       </c>
     </row>
@@ -43476,7 +43658,7 @@
         <v>2560</v>
       </c>
       <c r="D12">
-        <f>B12*C12/3600</f>
+        <f t="shared" si="0"/>
         <v>1.0666666666666667</v>
       </c>
     </row>
@@ -43491,7 +43673,7 @@
         <v>500</v>
       </c>
       <c r="D13">
-        <f>B13*C13/3600</f>
+        <f t="shared" si="0"/>
         <v>0.69444444444444442</v>
       </c>
     </row>
@@ -43503,10 +43685,10 @@
         <f>SUM(B5:B13)</f>
         <v>552.70000000000005</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="1">
         <f>SUM(D5:D13)</f>
         <v>42.456614011111114</v>
       </c>

</xml_diff>